<commit_message>
calculate fraction of bud burst at the budding phase, updating the met and pheno data set
</commit_message>
<xml_diff>
--- a/Prototypes/Grapevine/Observations/Marlborough_Sauvignon_blanc_PhenologyObs.xlsx
+++ b/Prototypes/Grapevine/Observations/Marlborough_Sauvignon_blanc_PhenologyObs.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APSIM_Grapevine\Grapevine\Observations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ApsimX\Prototypes\Grapevine\Observations\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22152" windowHeight="9972"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -42,19 +42,19 @@
     <t>Grapevine.Phenology.VeraisonDOY.Value()</t>
   </si>
   <si>
-    <t>PhenoTestClimateSite1001.met</t>
+    <t>PhenoTestClimateSite1001_BRA.met</t>
   </si>
   <si>
-    <t>PhenoTestClimateSite1002.met</t>
+    <t>PhenoTestClimateSite1002_OYB.met</t>
   </si>
   <si>
-    <t>PhenoTestClimateSite1003.met</t>
+    <t>PhenoTestClimateSite1003_SEA.met</t>
   </si>
   <si>
-    <t>PhenoTestClimateSite1004.met</t>
+    <t>PhenoTestClimateSite1004_RPC.met</t>
   </si>
   <si>
-    <t>PhenoTestClimateSite1005.met</t>
+    <t>PhenoTestClimateSite1005_VLA.met</t>
   </si>
   <si>
     <t>Booker</t>
@@ -393,13 +393,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="G71" sqref="G71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -426,7 +428,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
@@ -449,7 +451,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
@@ -472,7 +474,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
@@ -495,7 +497,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
@@ -518,7 +520,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
@@ -541,7 +543,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
@@ -564,7 +566,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -587,7 +589,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
@@ -610,7 +612,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10" t="s">
@@ -633,7 +635,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>7</v>
       </c>
       <c r="B11" t="s">
@@ -656,7 +658,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>7</v>
       </c>
       <c r="B12" t="s">
@@ -679,7 +681,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>7</v>
       </c>
       <c r="B13" t="s">
@@ -702,7 +704,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>7</v>
       </c>
       <c r="B14" t="s">
@@ -725,7 +727,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>8</v>
       </c>
       <c r="B15" t="s">
@@ -748,7 +750,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>8</v>
       </c>
       <c r="B16" t="s">
@@ -771,7 +773,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>8</v>
       </c>
       <c r="B17" t="s">
@@ -794,7 +796,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>8</v>
       </c>
       <c r="B18" t="s">
@@ -817,7 +819,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>8</v>
       </c>
       <c r="B19" t="s">
@@ -840,7 +842,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>8</v>
       </c>
       <c r="B20" t="s">
@@ -863,7 +865,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>8</v>
       </c>
       <c r="B21" t="s">
@@ -886,7 +888,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>8</v>
       </c>
       <c r="B22" t="s">
@@ -909,7 +911,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>8</v>
       </c>
       <c r="B23" t="s">
@@ -932,7 +934,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>8</v>
       </c>
       <c r="B24" t="s">
@@ -955,7 +957,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>8</v>
       </c>
       <c r="B25" t="s">
@@ -978,7 +980,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>8</v>
       </c>
       <c r="B26" t="s">
@@ -1001,7 +1003,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>8</v>
       </c>
       <c r="B27" t="s">
@@ -1024,7 +1026,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>9</v>
       </c>
       <c r="B28" t="s">
@@ -1047,7 +1049,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+      <c r="A29" t="s">
         <v>9</v>
       </c>
       <c r="B29" t="s">
@@ -1070,7 +1072,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
         <v>9</v>
       </c>
       <c r="B30" t="s">
@@ -1093,7 +1095,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
+      <c r="A31" t="s">
         <v>9</v>
       </c>
       <c r="B31" t="s">
@@ -1116,7 +1118,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
+      <c r="A32" t="s">
         <v>9</v>
       </c>
       <c r="B32" t="s">
@@ -1139,7 +1141,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
+      <c r="A33" t="s">
         <v>9</v>
       </c>
       <c r="B33" t="s">
@@ -1162,7 +1164,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+      <c r="A34" t="s">
         <v>9</v>
       </c>
       <c r="B34" t="s">
@@ -1185,7 +1187,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+      <c r="A35" t="s">
         <v>9</v>
       </c>
       <c r="B35" t="s">
@@ -1208,7 +1210,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>9</v>
       </c>
       <c r="B36" t="s">
@@ -1231,7 +1233,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
+      <c r="A37" t="s">
         <v>9</v>
       </c>
       <c r="B37" t="s">
@@ -1254,7 +1256,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
+      <c r="A38" t="s">
         <v>9</v>
       </c>
       <c r="B38" t="s">
@@ -1277,7 +1279,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
+      <c r="A39" t="s">
         <v>9</v>
       </c>
       <c r="B39" t="s">
@@ -1300,7 +1302,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
+      <c r="A40" t="s">
         <v>9</v>
       </c>
       <c r="B40" t="s">
@@ -1323,7 +1325,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
+      <c r="A41" t="s">
         <v>10</v>
       </c>
       <c r="B41" t="s">
@@ -1346,7 +1348,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
+      <c r="A42" t="s">
         <v>10</v>
       </c>
       <c r="B42" t="s">
@@ -1369,7 +1371,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
+      <c r="A43" t="s">
         <v>10</v>
       </c>
       <c r="B43" t="s">
@@ -1392,7 +1394,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
+      <c r="A44" t="s">
         <v>10</v>
       </c>
       <c r="B44" t="s">
@@ -1415,7 +1417,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
+      <c r="A45" t="s">
         <v>10</v>
       </c>
       <c r="B45" t="s">
@@ -1438,7 +1440,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
+      <c r="A46" t="s">
         <v>10</v>
       </c>
       <c r="B46" t="s">
@@ -1461,7 +1463,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
+      <c r="A47" t="s">
         <v>10</v>
       </c>
       <c r="B47" t="s">
@@ -1484,7 +1486,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
+      <c r="A48" t="s">
         <v>10</v>
       </c>
       <c r="B48" t="s">
@@ -1507,7 +1509,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
+      <c r="A49" t="s">
         <v>10</v>
       </c>
       <c r="B49" t="s">
@@ -1530,7 +1532,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
+      <c r="A50" t="s">
         <v>10</v>
       </c>
       <c r="B50" t="s">
@@ -1553,7 +1555,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
+      <c r="A51" t="s">
         <v>10</v>
       </c>
       <c r="B51" t="s">
@@ -1576,7 +1578,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
+      <c r="A52" t="s">
         <v>10</v>
       </c>
       <c r="B52" t="s">
@@ -1599,7 +1601,7 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
+      <c r="A53" t="s">
         <v>10</v>
       </c>
       <c r="B53" t="s">
@@ -1622,7 +1624,7 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
+      <c r="A54" t="s">
         <v>11</v>
       </c>
       <c r="B54" t="s">
@@ -1645,7 +1647,7 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
+      <c r="A55" t="s">
         <v>11</v>
       </c>
       <c r="B55" t="s">
@@ -1668,7 +1670,7 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
+      <c r="A56" t="s">
         <v>11</v>
       </c>
       <c r="B56" t="s">
@@ -1691,7 +1693,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
+      <c r="A57" t="s">
         <v>11</v>
       </c>
       <c r="B57" t="s">
@@ -1714,7 +1716,7 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
+      <c r="A58" t="s">
         <v>11</v>
       </c>
       <c r="B58" t="s">
@@ -1737,7 +1739,7 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
+      <c r="A59" t="s">
         <v>11</v>
       </c>
       <c r="B59" t="s">
@@ -1760,7 +1762,7 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
+      <c r="A60" t="s">
         <v>11</v>
       </c>
       <c r="B60" t="s">
@@ -1783,7 +1785,7 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
+      <c r="A61" t="s">
         <v>11</v>
       </c>
       <c r="B61" t="s">
@@ -1806,7 +1808,7 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
+      <c r="A62" t="s">
         <v>11</v>
       </c>
       <c r="B62" t="s">
@@ -1829,7 +1831,7 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
+      <c r="A63" t="s">
         <v>11</v>
       </c>
       <c r="B63" t="s">

</xml_diff>

<commit_message>
start to optimize the phenology prediction
</commit_message>
<xml_diff>
--- a/Prototypes/Grapevine/Observations/Marlborough_Sauvignon_blanc_PhenologyObs.xlsx
+++ b/Prototypes/Grapevine/Observations/Marlborough_Sauvignon_blanc_PhenologyObs.xlsx
@@ -20,19 +20,19 @@
     <t>Site</t>
   </si>
   <si>
-    <t>Grapevine.Phenology.CurrentSeason.Value()</t>
-  </si>
-  <si>
-    <t>Grapevine.Phenology.CurrentStageName</t>
-  </si>
-  <si>
-    <t>Grapevine.Phenology.BudBurstDOY.Value()</t>
-  </si>
-  <si>
-    <t>Grapevine.Phenology.FloweringDOY.Value()</t>
-  </si>
-  <si>
-    <t>Grapevine.Phenology.VeraisonDOY.Value()</t>
+    <t>CurrentSeason</t>
+  </si>
+  <si>
+    <t>CurrentStageName</t>
+  </si>
+  <si>
+    <t>BudBurstDOY</t>
+  </si>
+  <si>
+    <t>FloweringDOY</t>
+  </si>
+  <si>
+    <t>VeraisonDOY</t>
   </si>
   <si>
     <t>PhenoTestClimateSite1001_BRA.met</t>

</xml_diff>